<commit_message>
Print and Label Code.
</commit_message>
<xml_diff>
--- a/APAC/FILES/Schema.xlsx
+++ b/APAC/FILES/Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ociusnetgroup-my.sharepoint.com/personal/mikko_caguiat_ociusnetgroup_com/Documents/WORKING FILES/HEXATRONICS/HEXATRONIC_TRAINING_FILES/Hexatronic/APAC/FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="453" documentId="8_{D03B9754-463D-46A2-93A0-7A66DA3AB091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F94987F2-C460-4EE6-BA01-4BDFDB9D3E03}"/>
+  <xr:revisionPtr revIDLastSave="459" documentId="8_{D03B9754-463D-46A2-93A0-7A66DA3AB091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E69B96F-E6B4-47DA-9279-F0636B1E7BF0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B35381D8-35D7-44C3-AA6E-8470BE9F5B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B35381D8-35D7-44C3-AA6E-8470BE9F5B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Hexatronic_USA" sheetId="2" r:id="rId1"/>
@@ -1567,7 +1567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1678,13 +1678,7 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -10507,8 +10501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960B2FE8-6394-477C-AF7E-3881110516EB}">
   <dimension ref="A1:I363"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
@@ -13764,12 +13758,12 @@
       <c r="F203" s="2"/>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A204" s="48"/>
-      <c r="B204" s="49"/>
+      <c r="A204" s="13"/>
+      <c r="B204" s="15"/>
       <c r="C204" s="2"/>
       <c r="D204" s="4"/>
-      <c r="E204" s="50"/>
-      <c r="F204" s="48"/>
+      <c r="E204" s="48"/>
+      <c r="F204" s="13"/>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="13"/>
@@ -15816,10 +15810,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF6E6F4-EBF4-4EB2-A0A4-94E78DB5560C}">
-  <dimension ref="C2:G9"/>
+  <dimension ref="C2:G15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15922,6 +15916,33 @@
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E9" s="25"/>
     </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>418.5</v>
+      </c>
+      <c r="D13">
+        <f>C13/C14</f>
+        <v>1.236154186973859</v>
+      </c>
+      <c r="E13">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>338.55</v>
+      </c>
+      <c r="E14">
+        <f>E13*C14</f>
+        <v>142191</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f>E14/C13</f>
+        <v>339.76344086021504</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>